<commit_message>
Preparing for V8.0 with some inprovments in terms of price pr unit
</commit_message>
<xml_diff>
--- a/V7.1/Price estemate.xlsx
+++ b/V7.1/Price estemate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6de3b1494c6c18d5/GitHub/Smoke Stopper/V7.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57468\OneDrive\GitHub\Smoke Stopper\V7.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="175">
   <si>
     <t>Ref-Des</t>
   </si>
@@ -555,6 +555,9 @@
   </si>
   <si>
     <t>Price komp pr:</t>
+  </si>
+  <si>
+    <t>Price pr print:</t>
   </si>
 </sst>
 </file>
@@ -643,8 +646,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -966,7 +969,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +979,7 @@
     <col min="3" max="3" width="46.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -993,13 +996,19 @@
       <c r="E2" s="3" t="s">
         <v>173</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" s="11">
         <f>SUM(E5:E33)</f>
         <v>49.907000000000004</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="11">
+        <f>SUM(F5:F33)</f>
+        <v>51.87700000000001</v>
+      </c>
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1032,7 +1041,11 @@
       <c r="D5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="13">
+        <f>E5*A5</f>
         <v>0.6</v>
       </c>
     </row>
@@ -1049,7 +1062,11 @@
       <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" ref="F6:F33" si="0">E6*A6</f>
         <v>0.1</v>
       </c>
     </row>
@@ -1066,7 +1083,11 @@
       <c r="D7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
     </row>
@@ -1083,7 +1104,11 @@
       <c r="D8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
+        <v>2.6</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
     </row>
@@ -1100,7 +1125,11 @@
       <c r="D9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
@@ -1117,7 +1146,11 @@
       <c r="D10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
     </row>
@@ -1134,7 +1167,11 @@
       <c r="D11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1151,7 +1188,11 @@
       <c r="D12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
+        <v>2.7</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
     </row>
@@ -1168,7 +1209,11 @@
       <c r="D13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -1185,7 +1230,11 @@
       <c r="D14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1202,8 +1251,12 @@
       <c r="D15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>1.3</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1219,11 +1272,15 @@
       <c r="D16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="13">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>6</v>
       </c>
@@ -1236,11 +1293,15 @@
       <c r="D17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="13">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>3</v>
       </c>
@@ -1253,11 +1314,15 @@
       <c r="D18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="13">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>1</v>
       </c>
@@ -1270,11 +1335,15 @@
       <c r="D19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="13">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>1</v>
       </c>
@@ -1287,11 +1356,15 @@
       <c r="D20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="13">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>1</v>
       </c>
@@ -1304,11 +1377,15 @@
       <c r="D21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>1</v>
       </c>
@@ -1321,11 +1398,15 @@
       <c r="D22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="13">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>2</v>
       </c>
@@ -1338,11 +1419,15 @@
       <c r="D23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="13">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>1</v>
       </c>
@@ -1355,11 +1440,15 @@
       <c r="D24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="12">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="13">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>2</v>
       </c>
@@ -1372,11 +1461,15 @@
       <c r="D25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="12">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="13">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>1</v>
       </c>
@@ -1389,11 +1482,15 @@
       <c r="D26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="12">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="13">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>1</v>
       </c>
@@ -1406,11 +1503,15 @@
       <c r="D27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>1</v>
       </c>
@@ -1423,11 +1524,15 @@
       <c r="D28" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>1</v>
       </c>
@@ -1440,11 +1545,15 @@
       <c r="D29" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="12">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="13">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>1</v>
       </c>
@@ -1457,11 +1566,15 @@
       <c r="D30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>1</v>
       </c>
@@ -1474,11 +1587,15 @@
       <c r="D31" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>1</v>
       </c>
@@ -1491,11 +1608,15 @@
       <c r="D32" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="12">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="13">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>1</v>
       </c>
@@ -1508,11 +1629,15 @@
       <c r="D33" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="12">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="13">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
     </row>

</xml_diff>